<commit_message>
Adjust movetypes and movetype selection
</commit_message>
<xml_diff>
--- a/parameter/Takzeit_overview.xlsx
+++ b/parameter/Takzeit_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q517174\PycharmProjects\Optiflex\parameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8758B5-DE1B-4034-BE0F-27321AF10903}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6D8525-6258-4112-AA22-A2822D4AD940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3469,7 +3469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98CEFD0C-7A76-4D79-9CDA-EA74D2BB3CC5}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -5072,8 +5072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E24AD2-58D9-47FE-AC4F-FC115E5112C1}">
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5131,7 +5131,7 @@
         <v>50</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -5166,7 +5166,7 @@
         <v>50</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5201,7 +5201,7 @@
         <v>50</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -5236,7 +5236,7 @@
         <v>50</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -5271,7 +5271,7 @@
         <v>50</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -5306,7 +5306,7 @@
         <v>50</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -5341,7 +5341,7 @@
         <v>50</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -5376,7 +5376,7 @@
         <v>50</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -5411,7 +5411,7 @@
         <v>50</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -5446,7 +5446,7 @@
         <v>50</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -5481,7 +5481,7 @@
         <v>50</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -5516,7 +5516,7 @@
         <v>50</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -5551,7 +5551,7 @@
         <v>50</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -5586,7 +5586,7 @@
         <v>50</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -5621,7 +5621,7 @@
         <v>50</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -5656,7 +5656,7 @@
         <v>50</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -5691,7 +5691,7 @@
         <v>50</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -5726,7 +5726,7 @@
         <v>50</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -5761,7 +5761,7 @@
         <v>50</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -5796,7 +5796,7 @@
         <v>50</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -5831,7 +5831,7 @@
         <v>50</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -5866,7 +5866,7 @@
         <v>50</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -5901,7 +5901,7 @@
         <v>50</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -5936,7 +5936,7 @@
         <v>50</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -5971,7 +5971,7 @@
         <v>50</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -6006,7 +6006,7 @@
         <v>50</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -6041,7 +6041,7 @@
         <v>50</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -6076,7 +6076,7 @@
         <v>50</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -6111,7 +6111,7 @@
         <v>50</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -6356,7 +6356,7 @@
         <v>50</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -6391,7 +6391,7 @@
         <v>50</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -6426,7 +6426,7 @@
         <v>50</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -6461,7 +6461,7 @@
         <v>50</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -6496,7 +6496,7 @@
         <v>50</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -6601,7 +6601,7 @@
         <v>50</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -6636,7 +6636,7 @@
         <v>50</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -6671,7 +6671,7 @@
         <v>50</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -6706,7 +6706,7 @@
         <v>50</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -6741,7 +6741,7 @@
         <v>50</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -6776,7 +6776,7 @@
         <v>50</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -6811,7 +6811,7 @@
         <v>50</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -6846,7 +6846,7 @@
         <v>50</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -6881,7 +6881,7 @@
         <v>50</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -6916,7 +6916,7 @@
         <v>50</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -6951,7 +6951,7 @@
         <v>50</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -6986,7 +6986,7 @@
         <v>50</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -7021,7 +7021,7 @@
         <v>50</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -7056,7 +7056,7 @@
         <v>50</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -7091,7 +7091,7 @@
         <v>50</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -7126,7 +7126,7 @@
         <v>50</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -7161,7 +7161,7 @@
         <v>50</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -7196,7 +7196,7 @@
         <v>50</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -7231,7 +7231,7 @@
         <v>50</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -7266,7 +7266,7 @@
         <v>50</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -7301,7 +7301,7 @@
         <v>50</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -7336,7 +7336,7 @@
         <v>50</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -7371,7 +7371,7 @@
         <v>50</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -7406,7 +7406,7 @@
         <v>50</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -7441,7 +7441,7 @@
         <v>50</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -7476,7 +7476,7 @@
         <v>50</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -7511,7 +7511,7 @@
         <v>50</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -7546,7 +7546,7 @@
         <v>50</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -7581,7 +7581,7 @@
         <v>50</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -7616,7 +7616,7 @@
         <v>50</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -7651,7 +7651,7 @@
         <v>50</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -7686,7 +7686,7 @@
         <v>50</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -7721,7 +7721,7 @@
         <v>50</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -7756,7 +7756,7 @@
         <v>50</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -7791,7 +7791,7 @@
         <v>50</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -7826,7 +7826,7 @@
         <v>50</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="F79">
         <v>0</v>

</xml_diff>

<commit_message>
Write output pickle file
</commit_message>
<xml_diff>
--- a/parameter/Takzeit_overview.xlsx
+++ b/parameter/Takzeit_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\q517174\PycharmProjects\Optiflex\parameter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6D8525-6258-4112-AA22-A2822D4AD940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D408CB26-23C2-4CBB-8E14-73EA94D1F391}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="11265" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,22 +591,22 @@
       <selection sqref="A1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7265625" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" customWidth="1"/>
-    <col min="5" max="5" width="16.54296875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="21.1796875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="20.453125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -682,7 +682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -720,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -758,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -796,7 +796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -834,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -872,7 +872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -986,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1214,7 +1214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -2012,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -2316,7 +2316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>17</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>17</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>17</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>17</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>26</v>
       </c>
@@ -3000,7 +3000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>26</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>26</v>
       </c>
@@ -3076,7 +3076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>26</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>27</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>27</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>27</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>27</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>28</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>28</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -3473,12 +3473,12 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -3598,7 +3598,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3858,7 +3858,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -3878,7 +3878,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -4038,7 +4038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -4138,7 +4138,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -4158,7 +4158,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -4218,7 +4218,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -4318,7 +4318,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -4338,7 +4338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -4438,7 +4438,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -4478,7 +4478,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -4498,7 +4498,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -4558,7 +4558,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -4578,7 +4578,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -4618,7 +4618,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -4638,7 +4638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>29</v>
       </c>
@@ -4678,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>29</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -4818,7 +4818,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -4858,7 +4858,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>26</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>27</v>
       </c>
@@ -4898,7 +4898,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>27</v>
       </c>
@@ -4918,7 +4918,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>27</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>27</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>28</v>
       </c>
@@ -5018,7 +5018,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>28</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>28</v>
       </c>
@@ -5072,17 +5072,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0E24AD2-58D9-47FE-AC4F-FC115E5112C1}">
   <dimension ref="A1:K79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N78" sqref="N78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="11" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5117,7 +5117,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5125,13 +5125,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -5152,7 +5152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5160,13 +5160,13 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5187,7 +5187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -5195,13 +5195,13 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -5222,7 +5222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -5230,13 +5230,13 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -5257,7 +5257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -5265,13 +5265,13 @@
         <v>2</v>
       </c>
       <c r="C6">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -5292,7 +5292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -5300,13 +5300,13 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -5327,7 +5327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5335,13 +5335,13 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -5362,7 +5362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -5370,13 +5370,13 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -5397,7 +5397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -5405,13 +5405,13 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -5432,7 +5432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -5440,13 +5440,13 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -5467,7 +5467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -5475,13 +5475,13 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -5502,7 +5502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -5510,13 +5510,13 @@
         <v>2</v>
       </c>
       <c r="C13">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -5537,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -5545,13 +5545,13 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -5572,7 +5572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -5580,13 +5580,13 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -5607,7 +5607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5615,13 +5615,13 @@
         <v>5</v>
       </c>
       <c r="C16">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -5642,7 +5642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -5650,13 +5650,13 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -5677,7 +5677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -5685,13 +5685,13 @@
         <v>2</v>
       </c>
       <c r="C18">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -5712,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -5720,13 +5720,13 @@
         <v>3</v>
       </c>
       <c r="C19">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -5747,7 +5747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -5755,13 +5755,13 @@
         <v>4</v>
       </c>
       <c r="C20">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -5782,7 +5782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -5790,13 +5790,13 @@
         <v>5</v>
       </c>
       <c r="C21">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -5817,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -5825,13 +5825,13 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -5852,7 +5852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -5860,13 +5860,13 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -5887,7 +5887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -5895,13 +5895,13 @@
         <v>2</v>
       </c>
       <c r="C24">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -5922,7 +5922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -5930,13 +5930,13 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -5957,7 +5957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -5965,13 +5965,13 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -5992,7 +5992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -6000,13 +6000,13 @@
         <v>3</v>
       </c>
       <c r="C27">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -6027,7 +6027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
@@ -6035,13 +6035,13 @@
         <v>2</v>
       </c>
       <c r="C28">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -6062,7 +6062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -6070,13 +6070,13 @@
         <v>1</v>
       </c>
       <c r="C29">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -6097,7 +6097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -6105,13 +6105,13 @@
         <v>2</v>
       </c>
       <c r="C30">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -6132,7 +6132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -6202,7 +6202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>21</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>21</v>
       </c>
@@ -6342,7 +6342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -6350,13 +6350,13 @@
         <v>1</v>
       </c>
       <c r="C37">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -6377,7 +6377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -6385,13 +6385,13 @@
         <v>2</v>
       </c>
       <c r="C38">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -6412,7 +6412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -6420,13 +6420,13 @@
         <v>3</v>
       </c>
       <c r="C39">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -6447,7 +6447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -6455,13 +6455,13 @@
         <v>4</v>
       </c>
       <c r="C40">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -6482,7 +6482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -6490,13 +6490,13 @@
         <v>5</v>
       </c>
       <c r="C41">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -6517,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>22</v>
       </c>
@@ -6525,7 +6525,7 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -6552,7 +6552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>7</v>
       </c>
       <c r="C43">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -6587,7 +6587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -6595,13 +6595,13 @@
         <v>1</v>
       </c>
       <c r="C44">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -6622,7 +6622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -6630,13 +6630,13 @@
         <v>2</v>
       </c>
       <c r="C45">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -6657,7 +6657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -6665,13 +6665,13 @@
         <v>3</v>
       </c>
       <c r="C46">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -6692,7 +6692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>23</v>
       </c>
@@ -6700,13 +6700,13 @@
         <v>4</v>
       </c>
       <c r="C47">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -6727,7 +6727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>24</v>
       </c>
@@ -6735,13 +6735,13 @@
         <v>1</v>
       </c>
       <c r="C48">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -6762,7 +6762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -6770,13 +6770,13 @@
         <v>2</v>
       </c>
       <c r="C49">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -6797,7 +6797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -6805,13 +6805,13 @@
         <v>3</v>
       </c>
       <c r="C50">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -6832,7 +6832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>24</v>
       </c>
@@ -6840,13 +6840,13 @@
         <v>4</v>
       </c>
       <c r="C51">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -6867,7 +6867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>24</v>
       </c>
@@ -6875,13 +6875,13 @@
         <v>5</v>
       </c>
       <c r="C52">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -6902,7 +6902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>25</v>
       </c>
@@ -6910,13 +6910,13 @@
         <v>1</v>
       </c>
       <c r="C53">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E53">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -6937,7 +6937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -6945,13 +6945,13 @@
         <v>2</v>
       </c>
       <c r="C54">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -6972,7 +6972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -6980,13 +6980,13 @@
         <v>3</v>
       </c>
       <c r="C55">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -7007,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -7015,13 +7015,13 @@
         <v>4</v>
       </c>
       <c r="C56">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -7042,7 +7042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>25</v>
       </c>
@@ -7050,13 +7050,13 @@
         <v>5</v>
       </c>
       <c r="C57">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -7077,7 +7077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -7085,13 +7085,13 @@
         <v>1</v>
       </c>
       <c r="C58">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -7112,7 +7112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>29</v>
       </c>
@@ -7120,13 +7120,13 @@
         <v>2</v>
       </c>
       <c r="C59">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -7147,7 +7147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>29</v>
       </c>
@@ -7155,13 +7155,13 @@
         <v>3</v>
       </c>
       <c r="C60">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -7182,7 +7182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>29</v>
       </c>
@@ -7190,13 +7190,13 @@
         <v>4</v>
       </c>
       <c r="C61">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E61">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -7217,7 +7217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>17</v>
       </c>
@@ -7225,13 +7225,13 @@
         <v>1</v>
       </c>
       <c r="C62">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -7252,7 +7252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -7260,13 +7260,13 @@
         <v>2</v>
       </c>
       <c r="C63">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F63">
         <v>0</v>
@@ -7287,7 +7287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>17</v>
       </c>
@@ -7295,13 +7295,13 @@
         <v>3</v>
       </c>
       <c r="C64">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D64">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E64">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F64">
         <v>0</v>
@@ -7322,7 +7322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>17</v>
       </c>
@@ -7330,13 +7330,13 @@
         <v>4</v>
       </c>
       <c r="C65">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F65">
         <v>0</v>
@@ -7357,7 +7357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -7365,13 +7365,13 @@
         <v>5</v>
       </c>
       <c r="C66">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F66">
         <v>0</v>
@@ -7392,7 +7392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>26</v>
       </c>
@@ -7400,13 +7400,13 @@
         <v>1</v>
       </c>
       <c r="C67">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -7427,7 +7427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>26</v>
       </c>
@@ -7435,13 +7435,13 @@
         <v>2</v>
       </c>
       <c r="C68">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E68">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F68">
         <v>0</v>
@@ -7462,7 +7462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>26</v>
       </c>
@@ -7470,13 +7470,13 @@
         <v>3</v>
       </c>
       <c r="C69">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -7497,7 +7497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>26</v>
       </c>
@@ -7505,13 +7505,13 @@
         <v>4</v>
       </c>
       <c r="C70">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F70">
         <v>0</v>
@@ -7532,7 +7532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>27</v>
       </c>
@@ -7540,13 +7540,13 @@
         <v>1</v>
       </c>
       <c r="C71">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -7567,7 +7567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>27</v>
       </c>
@@ -7575,13 +7575,13 @@
         <v>4</v>
       </c>
       <c r="C72">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -7602,7 +7602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>27</v>
       </c>
@@ -7610,13 +7610,13 @@
         <v>5</v>
       </c>
       <c r="C73">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F73">
         <v>0</v>
@@ -7637,7 +7637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>27</v>
       </c>
@@ -7645,13 +7645,13 @@
         <v>6</v>
       </c>
       <c r="C74">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -7672,7 +7672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>28</v>
       </c>
@@ -7680,13 +7680,13 @@
         <v>1</v>
       </c>
       <c r="C75">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D75">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -7707,7 +7707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>28</v>
       </c>
@@ -7715,13 +7715,13 @@
         <v>2</v>
       </c>
       <c r="C76">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E76">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -7742,7 +7742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>28</v>
       </c>
@@ -7750,13 +7750,13 @@
         <v>3</v>
       </c>
       <c r="C77">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F77">
         <v>0</v>
@@ -7777,7 +7777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>28</v>
       </c>
@@ -7785,13 +7785,13 @@
         <v>4</v>
       </c>
       <c r="C78">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E78">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -7812,7 +7812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>28</v>
       </c>
@@ -7820,13 +7820,13 @@
         <v>5</v>
       </c>
       <c r="C79">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="F79">
         <v>0</v>

</xml_diff>